<commit_message>
Add more parameters to AccountBook.getBalance().
</commit_message>
<xml_diff>
--- a/MoneyTracking.xlsx
+++ b/MoneyTracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -91,7 +91,28 @@
     <t>99 Ranch</t>
   </si>
   <si>
+    <t>Chick-Fil-A</t>
+  </si>
+  <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>168 Market</t>
+  </si>
+  <si>
+    <t>Shopping &amp; Entertainment</t>
+  </si>
+  <si>
+    <t>FFXIV</t>
   </si>
   <si>
     <t>Saving</t>
@@ -101,6 +122,12 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>NTD</t>
+  </si>
+  <si>
+    <t>台北富邦</t>
   </si>
   <si>
     <t>FromBank</t>
@@ -136,15 +163,6 @@
     <t>Income Catagory</t>
   </si>
   <si>
-    <t>NTD</t>
-  </si>
-  <si>
-    <t>台北富邦</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
     <t>Deposits</t>
   </si>
   <si>
@@ -152,9 +170,6 @@
   </si>
   <si>
     <t>Interest</t>
-  </si>
-  <si>
-    <t>Shopping &amp; Entertainment</t>
   </si>
   <si>
     <t>Cash,Check &amp; Misc</t>
@@ -729,7 +744,7 @@
       <c r="G9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
@@ -756,7 +771,7 @@
       <c r="G10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
@@ -809,7 +824,7 @@
       <c r="G12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
         <v>13</v>
       </c>
@@ -836,57 +851,144 @@
       <c r="G13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="I13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="A14" s="3">
+        <v>43992.0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4">
+        <v>15.93</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="3">
+        <v>43993.0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4">
+        <v>21.75</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="I15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="3">
+        <v>43993.0</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4">
+        <v>66.02</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="I16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="A17" s="3">
+        <v>43993.0</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4">
+        <v>23.11</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="A18" s="3">
+        <v>43994.0</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4">
+        <v>14.99</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5"/>
@@ -9726,30 +9828,39 @@
       <c r="F1000" s="5"/>
       <c r="I1000" s="5"/>
     </row>
+    <row r="1001">
+      <c r="A1001" s="5"/>
+      <c r="B1001" s="5"/>
+      <c r="C1001" s="5"/>
+      <c r="D1001" s="5"/>
+      <c r="E1001" s="5"/>
+      <c r="F1001" s="5"/>
+      <c r="I1001" s="5"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I1000">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I1001">
       <formula1>Items!$F$2:$F$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1000">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1001">
       <formula1>"Home &amp; Utilities,Transportation,Groceries,Restaurants &amp; Dining,Shopping &amp; Entertainment,Cash,Check &amp; Misc,Finance,Init,Transfer"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="B2">
       <formula1>Items!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1000">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1001">
       <formula1>Items!$C$2:$C$1000</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1000">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1001">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B3:B1000">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B1001">
       <formula1>"USD,NTD"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1000">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1001">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1001">
       <formula1>Items!$B$2:$B$1000</formula1>
     </dataValidation>
   </dataValidations>
@@ -9847,7 +9958,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4">
         <v>18000.44</v>
@@ -9874,27 +9985,55 @@
         <v>1511.51</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="3">
+        <v>43986.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4">
+        <v>4614.0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="A6" s="3">
+        <v>43994.0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2736.82</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5"/>
@@ -17856,36 +17995,44 @@
       <c r="E1001" s="5"/>
       <c r="F1001" s="5"/>
     </row>
+    <row r="1002">
+      <c r="A1002" s="5"/>
+      <c r="B1002" s="5"/>
+      <c r="C1002" s="5"/>
+      <c r="D1002" s="5"/>
+      <c r="E1002" s="5"/>
+      <c r="F1002" s="5"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1000">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1001">
       <formula1>Items!$E$2:$E$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B1000">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B1001">
       <formula1>Items!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1000">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1001">
       <formula1>Items!$C$2:$C$1000</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1001">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1002">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C1001">
+    <dataValidation type="list" allowBlank="1" sqref="C1002">
       <formula1>"BOA,台北富邦"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B1001">
+    <dataValidation type="list" allowBlank="1" sqref="B1002">
       <formula1>"USD,NTD"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1001">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1002">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1001">
       <formula1>Items!$B$2:$B$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F1001">
+    <dataValidation type="list" allowBlank="1" sqref="F1002">
       <formula1>"Paycheck/Salary,Deposits,Interest,Init,Transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D1001">
+    <dataValidation type="list" allowBlank="1" sqref="D1002">
       <formula1>"Checking,Saving,CreditCard,Cash"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17908,28 +18055,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -17966,8 +18113,8 @@
       <c r="I2" s="4">
         <v>418.87</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>37</v>
+      <c r="J2" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>13</v>
@@ -27012,10 +27159,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -27055,7 +27202,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
@@ -27063,24 +27210,24 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -27089,12 +27236,12 @@
         <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
@@ -27105,17 +27252,17 @@
     </row>
     <row r="6">
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="D7" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="D8" s="10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Add jupyter notebook to make statistics.
</commit_message>
<xml_diff>
--- a/MoneyTracking.xlsx
+++ b/MoneyTracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -283,6 +283,12 @@
     <t>Amazon</t>
   </si>
   <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>0.16 - 0.04 Federal withholding</t>
+  </si>
+  <si>
     <t>Deposits</t>
   </si>
   <si>
@@ -295,9 +301,6 @@
     <t>Home (20000 - 20 - 15 wire transfer fee)</t>
   </si>
   <si>
-    <t>Interest</t>
-  </si>
-  <si>
     <t>0.17 - 0.04 Federal withholding</t>
   </si>
   <si>
@@ -305,6 +308,12 @@
   </si>
   <si>
     <t>Home (30000 - 20  - 15 wire transfer fee)</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Redeem cash rewards</t>
   </si>
   <si>
     <t>FromBank</t>
@@ -399,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -415,9 +424,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
@@ -3059,7 +3065,7 @@
       <c r="F93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G93" s="6" t="s">
+      <c r="G93" s="4" t="s">
         <v>73</v>
       </c>
       <c r="I93" s="4"/>
@@ -3293,7 +3299,7 @@
       <c r="F102" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G102" s="6" t="s">
+      <c r="G102" s="4" t="s">
         <v>30</v>
       </c>
       <c r="I102" s="4" t="s">
@@ -3305,7 +3311,7 @@
     </row>
     <row r="103">
       <c r="A103" s="3">
-        <v>44051.0</v>
+        <v>44050.0</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>9</v>
@@ -3317,13 +3323,13 @@
         <v>11</v>
       </c>
       <c r="E103" s="4">
-        <v>22.3</v>
+        <v>31.43</v>
       </c>
       <c r="F103" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G103" s="4" t="s">
-        <v>81</v>
+      <c r="G103" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>13</v>
@@ -3343,13 +3349,13 @@
         <v>11</v>
       </c>
       <c r="E104" s="4">
-        <v>111.54</v>
+        <v>22.3</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>13</v>
@@ -3369,21 +3375,21 @@
         <v>11</v>
       </c>
       <c r="E105" s="4">
-        <v>11.19</v>
+        <v>111.54</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="7">
-        <v>44052.0</v>
+      <c r="A106" s="3">
+        <v>44051.0</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>9</v>
@@ -3395,19 +3401,16 @@
         <v>11</v>
       </c>
       <c r="E106" s="4">
-        <v>45.1</v>
+        <v>11.19</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="I106" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="J106" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="107">
@@ -3421,22 +3424,27 @@
         <v>10</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="E107" s="4">
-        <v>205.0</v>
+        <v>45.1</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G107" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I107" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J107" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="3">
-        <v>44053.0</v>
+        <v>44052.0</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>9</v>
@@ -3445,20 +3453,18 @@
         <v>10</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E108" s="4">
-        <v>28.77</v>
+        <v>205.0</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I108" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="I108" s="4"/>
     </row>
     <row r="109">
       <c r="A109" s="3">
@@ -3474,13 +3480,13 @@
         <v>11</v>
       </c>
       <c r="E109" s="4">
-        <v>70.5</v>
+        <v>28.77</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>13</v>
@@ -3488,7 +3494,7 @@
     </row>
     <row r="110">
       <c r="A110" s="3">
-        <v>44054.0</v>
+        <v>44053.0</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>9</v>
@@ -3500,13 +3506,13 @@
         <v>11</v>
       </c>
       <c r="E110" s="4">
-        <v>48.5</v>
+        <v>70.5</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="I110" s="4" t="s">
         <v>13</v>
@@ -3526,26 +3532,43 @@
         <v>11</v>
       </c>
       <c r="E111" s="4">
-        <v>32.83</v>
+        <v>48.5</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="I111" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="5"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="I112" s="5"/>
+      <c r="A112" s="3">
+        <v>44054.0</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" s="4">
+        <v>32.83</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="5"/>
@@ -11620,30 +11643,39 @@
       <c r="F1009" s="5"/>
       <c r="I1009" s="5"/>
     </row>
+    <row r="1010">
+      <c r="A1010" s="5"/>
+      <c r="B1010" s="5"/>
+      <c r="C1010" s="5"/>
+      <c r="D1010" s="5"/>
+      <c r="E1010" s="5"/>
+      <c r="F1010" s="5"/>
+      <c r="I1010" s="5"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I1009">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I1010">
       <formula1>Items!$F$2:$F$1000</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="B2">
       <formula1>Items!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1009">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1010">
       <formula1>Items!$C$2:$C$1000</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A105 A107:A1009">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A106 A108:A1010">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B3:B1009">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B1010">
       <formula1>"USD,NTD"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E105 E107:E1009">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E106 E108:E1010">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1009">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1010">
       <formula1>Items!$B$2:$B$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1009">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1010">
       <formula1>Items!$D$2:$D$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -11727,8 +11759,8 @@
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="3">
@@ -11820,7 +11852,7 @@
     </row>
     <row r="7">
       <c r="A7" s="3">
-        <v>44008.0</v>
+        <v>44004.0</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>9</v>
@@ -11829,44 +11861,44 @@
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E7" s="4">
-        <v>2736.8</v>
+        <v>0.12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
-        <v>44012.0</v>
+        <v>44008.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="4">
-        <v>977.0</v>
+        <v>2736.8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3">
-        <v>44013.0</v>
+        <v>44012.0</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>32</v>
@@ -11878,41 +11910,41 @@
         <v>19</v>
       </c>
       <c r="E9" s="4">
-        <v>3036.0</v>
+        <v>977.0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
-        <v>44022.0</v>
+        <v>44013.0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="4">
-        <v>2736.82</v>
+        <v>3036.0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3">
-        <v>44032.0</v>
+        <v>44022.0</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
@@ -11924,18 +11956,18 @@
         <v>19</v>
       </c>
       <c r="E11" s="4">
-        <v>19965.0</v>
+        <v>2736.82</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3">
-        <v>44035.0</v>
+        <v>44032.0</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>9</v>
@@ -11944,13 +11976,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4">
-        <v>0.13</v>
+        <v>19965.0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>94</v>
@@ -11958,7 +11990,7 @@
     </row>
     <row r="13">
       <c r="A13" s="3">
-        <v>44036.0</v>
+        <v>44035.0</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
@@ -11967,21 +11999,21 @@
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E13" s="4">
-        <v>2736.81</v>
+        <v>0.13</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3">
-        <v>44042.0</v>
+        <v>44036.0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
@@ -11993,18 +12025,18 @@
         <v>19</v>
       </c>
       <c r="E14" s="4">
-        <v>10.55</v>
+        <v>2736.81</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3">
-        <v>44047.0</v>
+        <v>44042.0</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
@@ -12016,18 +12048,18 @@
         <v>19</v>
       </c>
       <c r="E15" s="4">
-        <v>29965.0</v>
+        <v>10.55</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3">
-        <v>44050.0</v>
+        <v>44047.0</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>9</v>
@@ -12039,30 +12071,60 @@
         <v>19</v>
       </c>
       <c r="E16" s="4">
+        <v>29965.0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3">
+        <v>44050.0</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4">
         <v>2736.8</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G17" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
     <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="3">
+        <v>44054.0</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4">
+        <v>23.15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5"/>
@@ -19936,36 +19998,44 @@
       <c r="E1002" s="5"/>
       <c r="F1002" s="5"/>
     </row>
+    <row r="1003">
+      <c r="A1003" s="5"/>
+      <c r="B1003" s="5"/>
+      <c r="C1003" s="5"/>
+      <c r="D1003" s="5"/>
+      <c r="E1003" s="5"/>
+      <c r="F1003" s="5"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1001">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1002">
       <formula1>Items!$E$2:$E$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B1001">
+    <dataValidation type="list" allowBlank="1" sqref="B2:B1002">
       <formula1>Items!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1001">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1002">
       <formula1>Items!$C$2:$C$1000</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1002">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1003">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C1002">
+    <dataValidation type="list" allowBlank="1" sqref="C1003">
       <formula1>"BOA,台北富邦"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B1002">
+    <dataValidation type="list" allowBlank="1" sqref="B1003">
       <formula1>"USD,NTD"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1002">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E1003">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1001">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1002">
       <formula1>Items!$B$2:$B$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F1002">
+    <dataValidation type="list" allowBlank="1" sqref="F1003">
       <formula1>"Paycheck/Salary,Deposits,Interest,Init,Transfer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D1002">
+    <dataValidation type="list" allowBlank="1" sqref="D1003">
       <formula1>"Checking,Saving,CreditCard,Cash"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19988,28 +20058,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -20047,7 +20117,7 @@
         <v>418.87</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>13</v>
@@ -20082,7 +20152,7 @@
         <v>844.0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K3" s="5"/>
     </row>
@@ -20115,7 +20185,7 @@
         <v>700.0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>13</v>
@@ -20180,7 +20250,7 @@
         <v>800.0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>13</v>
@@ -20275,7 +20345,7 @@
         <v>800.0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>13</v>
@@ -20300,7 +20370,9 @@
       <c r="F10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
@@ -20338,7 +20410,7 @@
         <v>500.0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>13</v>
@@ -29295,10 +29367,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -29334,7 +29406,7 @@
       <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -29358,7 +29430,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
@@ -29372,7 +29444,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -29393,6 +29465,9 @@
       <c r="D6" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="E6" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7">
       <c r="D7" s="4" t="s">
@@ -29400,7 +29475,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update spening from Evelyn's account.
</commit_message>
<xml_diff>
--- a/MoneyTracking.xlsx
+++ b/MoneyTracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -181,7 +181,19 @@
     <t>Wholefood</t>
   </si>
   <si>
+    <t>Credit Card - Evelyn</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>trash bag</t>
+  </si>
+  <si>
     <t>The Market at North PA</t>
+  </si>
+  <si>
+    <t>Keurig K-Mini Plus</t>
   </si>
   <si>
     <t>Saving</t>
@@ -191,6 +203,9 @@
   </si>
   <si>
     <t>Evergreen Pet Clinic</t>
+  </si>
+  <si>
+    <t>sifting litter box</t>
   </si>
   <si>
     <t>Sheng Kee Barkey</t>
@@ -226,7 +241,28 @@
     <t>5.99 + 0.17 foreign transaction fee</t>
   </si>
   <si>
+    <t>Macy's</t>
+  </si>
+  <si>
+    <t>Instant Pot Duo Nova</t>
+  </si>
+  <si>
+    <t>usb rechargeable laser pointer</t>
+  </si>
+  <si>
+    <t>wall small hole repair</t>
+  </si>
+  <si>
+    <t>cookware glass lib and hand truck</t>
+  </si>
+  <si>
     <t>Lemonade Insurance</t>
+  </si>
+  <si>
+    <t>Returning</t>
+  </si>
+  <si>
+    <t>Bakingware</t>
   </si>
   <si>
     <t>Costco Gas</t>
@@ -238,13 +274,16 @@
     <t>North Park</t>
   </si>
   <si>
-    <t>Credit Card - Evelyn</t>
-  </si>
-  <si>
     <t>Chewy</t>
   </si>
   <si>
     <t>Cat tree, shampoo, seat cover and e-collar</t>
+  </si>
+  <si>
+    <t>harness</t>
+  </si>
+  <si>
+    <t>Kitchen shear</t>
   </si>
   <si>
     <t>TjMax</t>
@@ -257,6 +296,12 @@
   </si>
   <si>
     <t>me, Evelyn and Mendy</t>
+  </si>
+  <si>
+    <t>adpotion fee</t>
+  </si>
+  <si>
+    <t>Lumi</t>
   </si>
   <si>
     <t>Tea Spoon</t>
@@ -274,13 +319,16 @@
     <t>Nintendo YsVIII</t>
   </si>
   <si>
+    <t xml:space="preserve">Keurig K-cups </t>
+  </si>
+  <si>
     <t>IKEA</t>
   </si>
   <si>
-    <t>Paycheck/Salary</t>
+    <t>Electric kettle and kitchen scoops</t>
   </si>
   <si>
-    <t>Amazon</t>
+    <t>Paycheck/Salary</t>
   </si>
   <si>
     <t>Interest</t>
@@ -357,7 +405,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -370,6 +418,9 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <name val="Arial"/>
     </font>
     <font/>
@@ -408,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -423,14 +474,29 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2203,29 +2269,49 @@
     </row>
     <row r="60">
       <c r="A60" s="3">
-        <v>44023.0</v>
-      </c>
-      <c r="B60" s="4" t="s">
+        <v>44022.0</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D60" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="4">
-        <v>6.24</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G60" s="4" t="s">
+      <c r="D60" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="I60" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E60" s="7">
+        <v>14.19</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H60" s="9"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
+      <c r="R60" s="9"/>
+      <c r="S60" s="9"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="9"/>
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+      <c r="Y60" s="9"/>
+      <c r="Z60" s="9"/>
+      <c r="AA60" s="9"/>
+      <c r="AB60" s="9"/>
     </row>
     <row r="61">
       <c r="A61" s="3">
@@ -2241,13 +2327,13 @@
         <v>11</v>
       </c>
       <c r="E61" s="4">
-        <v>35.59</v>
+        <v>6.24</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>13</v>
@@ -2267,13 +2353,13 @@
         <v>11</v>
       </c>
       <c r="E62" s="4">
-        <v>10.66</v>
+        <v>35.59</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>13</v>
@@ -2281,7 +2367,7 @@
     </row>
     <row r="63">
       <c r="A63" s="3">
-        <v>44024.0</v>
+        <v>44023.0</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>9</v>
@@ -2293,13 +2379,13 @@
         <v>11</v>
       </c>
       <c r="E63" s="4">
-        <v>14.99</v>
+        <v>10.66</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>13</v>
@@ -2319,13 +2405,13 @@
         <v>11</v>
       </c>
       <c r="E64" s="4">
-        <v>30.52</v>
+        <v>14.99</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>13</v>
@@ -2333,7 +2419,7 @@
     </row>
     <row r="65">
       <c r="A65" s="3">
-        <v>44025.0</v>
+        <v>44024.0</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>9</v>
@@ -2342,18 +2428,20 @@
         <v>10</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E65" s="4">
-        <v>88.67</v>
+        <v>30.52</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I65" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="3">
@@ -2369,19 +2457,19 @@
         <v>19</v>
       </c>
       <c r="E66" s="4">
-        <v>25.16</v>
+        <v>88.67</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I66" s="5"/>
     </row>
     <row r="67">
       <c r="A67" s="3">
-        <v>44029.0</v>
+        <v>44025.0</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>9</v>
@@ -2390,24 +2478,22 @@
         <v>10</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E67" s="4">
-        <v>74.31</v>
+        <v>25.16</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I67" s="5"/>
     </row>
     <row r="68">
       <c r="A68" s="3">
-        <v>44029.0</v>
+        <v>44026.0</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>9</v>
@@ -2416,22 +2502,22 @@
         <v>10</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E68" s="4">
-        <v>10000.0</v>
+        <v>87.39</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="I68" s="4"/>
     </row>
     <row r="69">
       <c r="A69" s="3">
-        <v>44030.0</v>
+        <v>44029.0</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>9</v>
@@ -2443,13 +2529,13 @@
         <v>11</v>
       </c>
       <c r="E69" s="4">
-        <v>50.0</v>
+        <v>74.31</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>13</v>
@@ -2457,7 +2543,7 @@
     </row>
     <row r="70">
       <c r="A70" s="3">
-        <v>44030.0</v>
+        <v>44029.0</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>9</v>
@@ -2466,24 +2552,22 @@
         <v>10</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="E70" s="4">
-        <v>35.59</v>
+        <v>10000.0</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I70" s="4"/>
     </row>
     <row r="71">
       <c r="A71" s="3">
-        <v>44031.0</v>
+        <v>44030.0</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>9</v>
@@ -2495,13 +2579,13 @@
         <v>11</v>
       </c>
       <c r="E71" s="4">
-        <v>8.69</v>
+        <v>50.0</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>13</v>
@@ -2509,7 +2593,7 @@
     </row>
     <row r="72">
       <c r="A72" s="3">
-        <v>44033.0</v>
+        <v>44030.0</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>9</v>
@@ -2521,13 +2605,13 @@
         <v>11</v>
       </c>
       <c r="E72" s="4">
-        <v>30.51</v>
+        <v>35.59</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>13</v>
@@ -2535,7 +2619,7 @@
     </row>
     <row r="73">
       <c r="A73" s="3">
-        <v>44033.0</v>
+        <v>44030.0</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>9</v>
@@ -2544,24 +2628,25 @@
         <v>10</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E73" s="4">
-        <v>11.0</v>
+        <v>18.39</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3">
-        <v>44033.0</v>
+        <v>44031.0</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>9</v>
@@ -2573,13 +2658,13 @@
         <v>11</v>
       </c>
       <c r="E74" s="4">
-        <v>5.99</v>
+        <v>8.69</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>13</v>
@@ -2587,7 +2672,7 @@
     </row>
     <row r="75">
       <c r="A75" s="3">
-        <v>44037.0</v>
+        <v>44033.0</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>9</v>
@@ -2599,13 +2684,13 @@
         <v>11</v>
       </c>
       <c r="E75" s="4">
-        <v>8.72</v>
+        <v>30.51</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>13</v>
@@ -2613,7 +2698,7 @@
     </row>
     <row r="76">
       <c r="A76" s="3">
-        <v>44037.0</v>
+        <v>44033.0</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>9</v>
@@ -2625,13 +2710,13 @@
         <v>11</v>
       </c>
       <c r="E76" s="4">
-        <v>55.17</v>
+        <v>11.0</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>13</v>
@@ -2639,7 +2724,7 @@
     </row>
     <row r="77">
       <c r="A77" s="3">
-        <v>44038.0</v>
+        <v>44033.0</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>9</v>
@@ -2651,13 +2736,13 @@
         <v>11</v>
       </c>
       <c r="E77" s="4">
-        <v>43.77</v>
+        <v>5.99</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>13</v>
@@ -2665,7 +2750,7 @@
     </row>
     <row r="78">
       <c r="A78" s="3">
-        <v>44038.0</v>
+        <v>44037.0</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>9</v>
@@ -2677,13 +2762,13 @@
         <v>11</v>
       </c>
       <c r="E78" s="4">
-        <v>61.13</v>
+        <v>8.72</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>13</v>
@@ -2691,7 +2776,7 @@
     </row>
     <row r="79">
       <c r="A79" s="3">
-        <v>44038.0</v>
+        <v>44037.0</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>9</v>
@@ -2703,13 +2788,13 @@
         <v>11</v>
       </c>
       <c r="E79" s="4">
-        <v>7.0</v>
+        <v>55.17</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>13</v>
@@ -2729,13 +2814,13 @@
         <v>11</v>
       </c>
       <c r="E80" s="4">
-        <v>28.6</v>
+        <v>43.77</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>13</v>
@@ -2755,13 +2840,13 @@
         <v>11</v>
       </c>
       <c r="E81" s="4">
-        <v>52.44</v>
+        <v>61.13</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>13</v>
@@ -2769,160 +2854,157 @@
     </row>
     <row r="82">
       <c r="A82" s="3">
-        <v>44039.0</v>
+        <v>44038.0</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E82" s="4">
-        <v>199.0</v>
+        <v>7.0</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I82" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="3">
-        <v>44039.0</v>
+        <v>44038.0</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E83" s="4">
-        <v>510.0</v>
+        <v>28.6</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I83" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="3">
-        <v>44039.0</v>
+        <v>44038.0</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E84" s="4">
-        <v>836.0</v>
+        <v>52.44</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I84" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="3">
         <v>44039.0</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E85" s="4">
-        <v>6.16</v>
+        <v>199.0</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I85" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J85" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="I85" s="5"/>
     </row>
     <row r="86">
       <c r="A86" s="3">
-        <v>44042.0</v>
+        <v>44039.0</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E86" s="4">
-        <v>5.0</v>
+        <v>510.0</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="I86" s="5"/>
     </row>
     <row r="87">
       <c r="A87" s="3">
-        <v>44042.0</v>
+        <v>44039.0</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E87" s="4">
-        <v>16.86</v>
+        <v>836.0</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I87" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="I87" s="5"/>
     </row>
     <row r="88">
       <c r="A88" s="3">
-        <v>44043.0</v>
+        <v>44039.0</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>9</v>
@@ -2931,22 +3013,27 @@
         <v>10</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E88" s="4">
-        <v>29.7</v>
+        <v>6.16</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I88" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="3">
-        <v>44043.0</v>
+        <v>44039.0</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>9</v>
@@ -2955,22 +3042,25 @@
         <v>10</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="E89" s="4">
-        <v>43.58</v>
+        <v>109.24</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I89" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="3">
-        <v>44043.0</v>
+        <v>44039.0</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>9</v>
@@ -2979,24 +3069,25 @@
         <v>10</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E90" s="4">
-        <v>23.6</v>
+        <v>14.19</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G90" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="I90" s="4" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I90" s="4"/>
+      <c r="J90" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3">
-        <v>44043.0</v>
+        <v>44040.0</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>9</v>
@@ -3005,24 +3096,25 @@
         <v>10</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E91" s="4">
-        <v>78.1</v>
+        <v>7.61</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I91" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I91" s="4"/>
+      <c r="J91" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3">
-        <v>44043.0</v>
+        <v>44040.0</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>9</v>
@@ -3031,24 +3123,25 @@
         <v>10</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E92" s="4">
-        <v>5.5</v>
+        <v>78.43</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I92" s="4"/>
+      <c r="J92" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3">
-        <v>44043.0</v>
+        <v>44042.0</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>9</v>
@@ -3057,22 +3150,24 @@
         <v>10</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E93" s="4">
-        <v>1853.46</v>
+        <v>5.0</v>
       </c>
       <c r="F93" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I93" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="3">
-        <v>44044.0</v>
+        <v>44042.0</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>9</v>
@@ -3084,13 +3179,13 @@
         <v>11</v>
       </c>
       <c r="E94" s="4">
-        <v>35.59</v>
+        <v>16.86</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>13</v>
@@ -3098,7 +3193,7 @@
     </row>
     <row r="95">
       <c r="A95" s="3">
-        <v>44044.0</v>
+        <v>44042.0</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>9</v>
@@ -3107,24 +3202,28 @@
         <v>10</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E95" s="4">
-        <v>7.16</v>
+        <v>29.7</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I95" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I95" s="5"/>
+      <c r="J95" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3">
-        <v>44045.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>9</v>
@@ -3136,19 +3235,19 @@
         <v>19</v>
       </c>
       <c r="E96" s="4">
-        <v>77.91</v>
+        <v>29.7</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I96" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="I96" s="5"/>
     </row>
     <row r="97">
       <c r="A97" s="3">
-        <v>44045.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>9</v>
@@ -3157,25 +3256,22 @@
         <v>10</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="E97" s="4">
-        <v>122.6</v>
+        <v>43.58</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="I97" s="5"/>
-      <c r="J97" s="4" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" s="3">
-        <v>44047.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>9</v>
@@ -3187,13 +3283,13 @@
         <v>11</v>
       </c>
       <c r="E98" s="4">
-        <v>30.47</v>
+        <v>23.6</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>13</v>
@@ -3201,7 +3297,7 @@
     </row>
     <row r="99">
       <c r="A99" s="3">
-        <v>44047.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>9</v>
@@ -3213,13 +3309,13 @@
         <v>11</v>
       </c>
       <c r="E99" s="4">
-        <v>37.44</v>
+        <v>78.1</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>13</v>
@@ -3227,7 +3323,7 @@
     </row>
     <row r="100">
       <c r="A100" s="3">
-        <v>44050.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>9</v>
@@ -3239,24 +3335,21 @@
         <v>11</v>
       </c>
       <c r="E100" s="4">
-        <v>52.46</v>
+        <v>5.5</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J100" s="4" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" s="3">
-        <v>44050.0</v>
+        <v>44043.0</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>9</v>
@@ -3265,24 +3358,22 @@
         <v>10</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E101" s="4">
-        <v>38.13</v>
+        <v>1853.46</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I101" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="I101" s="4"/>
     </row>
     <row r="102">
       <c r="A102" s="3">
-        <v>44050.0</v>
+        <v>44044.0</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>9</v>
@@ -3294,24 +3385,21 @@
         <v>11</v>
       </c>
       <c r="E102" s="4">
-        <v>43.87</v>
+        <v>35.59</v>
       </c>
       <c r="F102" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I102" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J102" s="4" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" s="3">
-        <v>44050.0</v>
+        <v>44044.0</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>9</v>
@@ -3323,13 +3411,13 @@
         <v>11</v>
       </c>
       <c r="E103" s="4">
-        <v>31.43</v>
+        <v>7.16</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>13</v>
@@ -3337,7 +3425,7 @@
     </row>
     <row r="104">
       <c r="A104" s="3">
-        <v>44051.0</v>
+        <v>44045.0</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>9</v>
@@ -3346,24 +3434,22 @@
         <v>10</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E104" s="4">
-        <v>22.3</v>
+        <v>77.91</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I104" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I104" s="4"/>
     </row>
     <row r="105">
       <c r="A105" s="3">
-        <v>44051.0</v>
+        <v>44045.0</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>9</v>
@@ -3372,24 +3458,25 @@
         <v>10</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E105" s="4">
-        <v>111.54</v>
+        <v>122.6</v>
       </c>
       <c r="F105" s="4" t="s">
         <v>50</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I105" s="4" t="s">
-        <v>13</v>
+        <v>86</v>
+      </c>
+      <c r="I105" s="5"/>
+      <c r="J105" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3">
-        <v>44051.0</v>
+        <v>44045.0</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>9</v>
@@ -3398,24 +3485,25 @@
         <v>10</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E106" s="4">
-        <v>11.19</v>
+        <v>16.37</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I106" s="4" t="s">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I106" s="4"/>
+      <c r="J106" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3">
-        <v>44052.0</v>
+        <v>44046.0</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>9</v>
@@ -3424,27 +3512,25 @@
         <v>10</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="E107" s="4">
-        <v>45.1</v>
+        <v>21.84</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G107" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I107" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I107" s="4"/>
       <c r="J107" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3">
-        <v>44052.0</v>
+        <v>44047.0</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>9</v>
@@ -3453,22 +3539,24 @@
         <v>10</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="E108" s="4">
-        <v>205.0</v>
+        <v>30.47</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I108" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="3">
-        <v>44053.0</v>
+        <v>44047.0</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>9</v>
@@ -3480,13 +3568,13 @@
         <v>11</v>
       </c>
       <c r="E109" s="4">
-        <v>28.77</v>
+        <v>37.44</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>13</v>
@@ -3494,7 +3582,7 @@
     </row>
     <row r="110">
       <c r="A110" s="3">
-        <v>44053.0</v>
+        <v>44050.0</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>9</v>
@@ -3506,21 +3594,24 @@
         <v>11</v>
       </c>
       <c r="E110" s="4">
-        <v>70.5</v>
+        <v>52.46</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="I110" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J110" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="3">
-        <v>44054.0</v>
+        <v>44050.0</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>9</v>
@@ -3532,13 +3623,13 @@
         <v>11</v>
       </c>
       <c r="E111" s="4">
-        <v>48.5</v>
+        <v>38.13</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="I111" s="4" t="s">
         <v>13</v>
@@ -3546,7 +3637,7 @@
     </row>
     <row r="112">
       <c r="A112" s="3">
-        <v>44054.0</v>
+        <v>44050.0</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>9</v>
@@ -3558,134 +3649,359 @@
         <v>11</v>
       </c>
       <c r="E112" s="4">
-        <v>32.83</v>
+        <v>43.87</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="J112" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="I113" s="5"/>
+      <c r="A113" s="3">
+        <v>44050.0</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" s="4">
+        <v>31.43</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="5"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="5"/>
-      <c r="I114" s="5"/>
+      <c r="A114" s="3">
+        <v>44050.0</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E114" s="4">
+        <v>125.0</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="5"/>
-      <c r="I115" s="5"/>
+      <c r="A115" s="3">
+        <v>44051.0</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="4">
+        <v>22.3</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I115" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" s="5"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="I116" s="5"/>
+      <c r="A116" s="3">
+        <v>44051.0</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="4">
+        <v>111.54</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I116" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="117">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="I117" s="5"/>
+      <c r="A117" s="3">
+        <v>44051.0</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="4">
+        <v>11.19</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I117" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="I118" s="5"/>
+      <c r="A118" s="3">
+        <v>44052.0</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E118" s="4">
+        <v>45.1</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I118" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J118" s="11" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="119">
-      <c r="A119" s="5"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="I119" s="5"/>
+      <c r="A119" s="3">
+        <v>44052.0</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E119" s="4">
+        <v>205.0</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="I119" s="4"/>
     </row>
     <row r="120">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="I120" s="5"/>
+      <c r="A120" s="3">
+        <v>44053.0</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E120" s="4">
+        <v>28.77</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="I120" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" s="5"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="I121" s="5"/>
+      <c r="A121" s="3">
+        <v>44053.0</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121" s="4">
+        <v>70.5</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I121" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="122">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="I122" s="5"/>
+      <c r="A122" s="3">
+        <v>44053.0</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E122" s="4">
+        <v>40.56</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I122" s="4"/>
     </row>
     <row r="123">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="I123" s="5"/>
+      <c r="A123" s="3">
+        <v>44054.0</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E123" s="4">
+        <v>48.5</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I123" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" s="5"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
-      <c r="F124" s="5"/>
-      <c r="I124" s="5"/>
+      <c r="A124" s="3">
+        <v>44054.0</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E124" s="4">
+        <v>32.83</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I124" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="125">
-      <c r="A125" s="5"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="5"/>
-      <c r="F125" s="5"/>
+      <c r="A125" s="3">
+        <v>44055.0</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E125" s="4">
+        <v>50.23</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="I125" s="5"/>
+      <c r="J125" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="5"/>
@@ -11652,30 +11968,138 @@
       <c r="F1010" s="5"/>
       <c r="I1010" s="5"/>
     </row>
+    <row r="1011">
+      <c r="A1011" s="5"/>
+      <c r="B1011" s="5"/>
+      <c r="C1011" s="5"/>
+      <c r="D1011" s="5"/>
+      <c r="E1011" s="5"/>
+      <c r="F1011" s="5"/>
+      <c r="I1011" s="5"/>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="5"/>
+      <c r="B1012" s="5"/>
+      <c r="C1012" s="5"/>
+      <c r="D1012" s="5"/>
+      <c r="E1012" s="5"/>
+      <c r="F1012" s="5"/>
+      <c r="I1012" s="5"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="5"/>
+      <c r="B1013" s="5"/>
+      <c r="C1013" s="5"/>
+      <c r="D1013" s="5"/>
+      <c r="E1013" s="5"/>
+      <c r="F1013" s="5"/>
+      <c r="I1013" s="5"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="5"/>
+      <c r="B1014" s="5"/>
+      <c r="C1014" s="5"/>
+      <c r="D1014" s="5"/>
+      <c r="E1014" s="5"/>
+      <c r="F1014" s="5"/>
+      <c r="I1014" s="5"/>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="5"/>
+      <c r="B1015" s="5"/>
+      <c r="C1015" s="5"/>
+      <c r="D1015" s="5"/>
+      <c r="E1015" s="5"/>
+      <c r="F1015" s="5"/>
+      <c r="I1015" s="5"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="5"/>
+      <c r="B1016" s="5"/>
+      <c r="C1016" s="5"/>
+      <c r="D1016" s="5"/>
+      <c r="E1016" s="5"/>
+      <c r="F1016" s="5"/>
+      <c r="I1016" s="5"/>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="5"/>
+      <c r="B1017" s="5"/>
+      <c r="C1017" s="5"/>
+      <c r="D1017" s="5"/>
+      <c r="E1017" s="5"/>
+      <c r="F1017" s="5"/>
+      <c r="I1017" s="5"/>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="5"/>
+      <c r="B1018" s="5"/>
+      <c r="C1018" s="5"/>
+      <c r="D1018" s="5"/>
+      <c r="E1018" s="5"/>
+      <c r="F1018" s="5"/>
+      <c r="I1018" s="5"/>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="5"/>
+      <c r="B1019" s="5"/>
+      <c r="C1019" s="5"/>
+      <c r="D1019" s="5"/>
+      <c r="E1019" s="5"/>
+      <c r="F1019" s="5"/>
+      <c r="I1019" s="5"/>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="5"/>
+      <c r="B1020" s="5"/>
+      <c r="C1020" s="5"/>
+      <c r="D1020" s="5"/>
+      <c r="E1020" s="5"/>
+      <c r="F1020" s="5"/>
+      <c r="I1020" s="5"/>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="5"/>
+      <c r="B1021" s="5"/>
+      <c r="C1021" s="5"/>
+      <c r="D1021" s="5"/>
+      <c r="E1021" s="5"/>
+      <c r="F1021" s="5"/>
+      <c r="I1021" s="5"/>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="5"/>
+      <c r="B1022" s="5"/>
+      <c r="C1022" s="5"/>
+      <c r="D1022" s="5"/>
+      <c r="E1022" s="5"/>
+      <c r="F1022" s="5"/>
+      <c r="I1022" s="5"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I1010">
+    <dataValidation type="list" allowBlank="1" sqref="I2:I1022">
       <formula1>Items!$F$2:$F$1000</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="B2">
       <formula1>Items!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1010">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1022">
       <formula1>Items!$C$2:$C$1000</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A106 A108:A1010">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A117 A119:A1022">
       <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B3:B1010">
+    <dataValidation type="list" allowBlank="1" sqref="B3:B1022">
       <formula1>"USD,NTD"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E106 E108:E1010">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" sqref="E2:E117 E119:E1022">
       <formula1>0.0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1010">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1022">
       <formula1>Items!$B$2:$B$1000</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1010">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F1022">
       <formula1>Items!$D$2:$D$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -11759,8 +12183,8 @@
       <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3">
       <c r="A3" s="3">
@@ -11773,7 +12197,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>18000.44</v>
@@ -11800,10 +12224,10 @@
         <v>1511.51</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -11844,10 +12268,10 @@
         <v>2736.82</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -11861,16 +12285,16 @@
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4">
         <v>0.12</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8">
@@ -11890,10 +12314,10 @@
         <v>2736.8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -11913,10 +12337,10 @@
         <v>977.0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
@@ -11936,10 +12360,10 @@
         <v>3036.0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11">
@@ -11959,10 +12383,10 @@
         <v>2736.82</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -11982,10 +12406,10 @@
         <v>19965.0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -11999,16 +12423,16 @@
         <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E13" s="4">
         <v>0.13</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14">
@@ -12028,10 +12452,10 @@
         <v>2736.81</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -12051,10 +12475,10 @@
         <v>10.55</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
@@ -12074,10 +12498,10 @@
         <v>29965.0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17">
@@ -12097,10 +12521,10 @@
         <v>2736.8</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
@@ -12117,13 +12541,13 @@
         <v>11</v>
       </c>
       <c r="E18" s="4">
-        <v>23.15</v>
+        <v>23.24</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>99</v>
+        <v>114</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19">
@@ -20058,28 +20482,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -20117,7 +20541,7 @@
         <v>418.87</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>13</v>
@@ -20152,7 +20576,7 @@
         <v>844.0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K3" s="5"/>
     </row>
@@ -20185,7 +20609,7 @@
         <v>700.0</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>13</v>
@@ -20211,7 +20635,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>9</v>
@@ -20250,7 +20674,7 @@
         <v>800.0</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>13</v>
@@ -20276,7 +20700,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>9</v>
@@ -20306,7 +20730,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>9</v>
@@ -20345,7 +20769,7 @@
         <v>800.0</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>13</v>
@@ -20368,10 +20792,10 @@
         <v>260.0</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>9</v>
@@ -20410,7 +20834,7 @@
         <v>500.0</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>13</v>
@@ -29367,10 +29791,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -29406,11 +29830,11 @@
       <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
@@ -29424,18 +29848,18 @@
         <v>33</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -29444,12 +29868,12 @@
         <v>16</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="4" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
@@ -29460,13 +29884,13 @@
     </row>
     <row r="6">
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
@@ -29475,8 +29899,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="D8" s="9" t="s">
-        <v>65</v>
+      <c r="D8" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9">

</xml_diff>